<commit_message>
Update DataModel、UI、 Export excl.
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
+++ b/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
@@ -58,10 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">总阻力  P </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>选型余压</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -226,6 +222,10 @@
       </rPr>
       <t>/h</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>选型全压</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -632,7 +632,7 @@
   <dimension ref="A1:W335"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -640,10 +640,11 @@
     <col min="1" max="1" width="8" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" style="6" customWidth="1"/>
     <col min="3" max="3" width="11.875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12" style="6" customWidth="1"/>
-    <col min="5" max="9" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="9" width="8" style="6" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="6.375" style="6" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="8" style="6" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="8" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.875" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.375" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="8" style="6" bestFit="1" customWidth="1"/>
@@ -659,40 +660,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>2</v>
@@ -719,10 +720,10 @@
         <v>9</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -741,29 +742,29 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
@@ -771,60 +772,60 @@
       <c r="B3" s="8"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -9129,12 +9130,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="G1:G2"/>
@@ -9143,6 +9138,12 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement model calculation (#452)
Co-authored-by: york <chenyue1991@sina.com>
Co-authored-by: Seven <85804174@qq.com>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
+++ b/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="防烟计算" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -631,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W335"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -9149,4 +9150,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A20:A26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update model block template file
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
+++ b/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="风机计算" sheetId="1" r:id="rId1"/>
     <sheet name="防烟计算" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -239,7 +239,7 @@
     <numFmt numFmtId="177" formatCode="0.0_ "/>
     <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +284,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -323,7 +330,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -346,6 +353,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -632,11 +640,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W335"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.875" style="6" customWidth="1"/>
@@ -657,46 +665,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -728,20 +736,20 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
       <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
@@ -769,8 +777,8 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>40</v>
@@ -9131,6 +9139,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="G1:G2"/>
@@ -9139,12 +9153,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9154,20 +9162,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A20:A26"/>
+  <dimension ref="A19:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="6.375" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="8"/>
+  </cols>
   <sheetData>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update FanCalc Excel template file 增加了末端预留风压列
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
+++ b/AutoLoader/Contents/Support/DesignData/FanCalc.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AE1D9A-88E2-4E0F-BEDD-E7E30D03986A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="风机计算" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>设备编号</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -230,11 +231,15 @@
     <t>选型全压</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>末端预留风压</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="0.0_ "/>
@@ -331,7 +336,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -358,10 +363,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 13" xfId="1"/>
+    <cellStyle name="常规 13" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -638,74 +646,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W335"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X335"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="6" customWidth="1"/>
     <col min="4" max="4" width="12" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="9" width="8" style="6" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="6.375" style="6" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="6" hidden="1" customWidth="1"/>
     <col min="11" max="12" width="8" style="6" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.75" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.375" style="6" customWidth="1"/>
-    <col min="24" max="16384" width="9" style="6"/>
+    <col min="20" max="20" width="8" style="6" customWidth="1"/>
+    <col min="21" max="21" width="7.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" style="6" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:24" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="1" t="s">
@@ -723,34 +732,37 @@
       <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
+    <row r="2" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
       <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
@@ -764,7 +776,7 @@
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="9" t="s">
         <v>13</v>
       </c>
       <c r="U2" s="1" t="s">
@@ -774,12 +786,15 @@
         <v>13</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+    <row r="3" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>40</v>
@@ -827,18 +842,19 @@
       <c r="S3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="9"/>
+      <c r="U3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="1"/>
+      <c r="X3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -862,8 +878,9 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X4" s="3"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -886,9 +903,10 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
-      <c r="W5" s="5"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W5" s="3"/>
+      <c r="X5" s="5"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -911,9 +929,10 @@
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="5"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W6" s="3"/>
+      <c r="X6" s="5"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -936,9 +955,10 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
-      <c r="W7" s="5"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W7" s="3"/>
+      <c r="X7" s="5"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -961,9 +981,10 @@
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
-      <c r="W8" s="5"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W8" s="3"/>
+      <c r="X8" s="5"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -986,9 +1007,10 @@
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
-      <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W9" s="3"/>
+      <c r="X9" s="5"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1012,8 +1034,9 @@
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X10" s="7"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1037,8 +1060,9 @@
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X11" s="7"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1062,8 +1086,9 @@
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X12" s="7"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1087,8 +1112,9 @@
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X13" s="7"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1112,8 +1138,9 @@
       <c r="U14" s="7"/>
       <c r="V14" s="7"/>
       <c r="W14" s="7"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X14" s="7"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1137,8 +1164,9 @@
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
       <c r="W15" s="7"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X15" s="7"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1162,8 +1190,9 @@
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X16" s="7"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1187,8 +1216,9 @@
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X17" s="7"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1212,8 +1242,9 @@
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18" s="7"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1237,8 +1268,9 @@
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X19" s="7"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1262,8 +1294,9 @@
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X20" s="7"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1287,8 +1320,9 @@
       <c r="U21" s="7"/>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X21" s="7"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1312,8 +1346,9 @@
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X22" s="7"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1337,8 +1372,9 @@
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X23" s="7"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1362,8 +1398,9 @@
       <c r="U24" s="7"/>
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X24" s="7"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1387,8 +1424,9 @@
       <c r="U25" s="7"/>
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X25" s="7"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1412,8 +1450,9 @@
       <c r="U26" s="7"/>
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X26" s="7"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1437,8 +1476,9 @@
       <c r="U27" s="7"/>
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X27" s="7"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1462,8 +1502,9 @@
       <c r="U28" s="7"/>
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X28" s="7"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1487,8 +1528,9 @@
       <c r="U29" s="7"/>
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X29" s="7"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1512,8 +1554,9 @@
       <c r="U30" s="7"/>
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X30" s="7"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1537,8 +1580,9 @@
       <c r="U31" s="7"/>
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X31" s="7"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1562,8 +1606,9 @@
       <c r="U32" s="7"/>
       <c r="V32" s="7"/>
       <c r="W32" s="7"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X32" s="7"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1587,8 +1632,9 @@
       <c r="U33" s="7"/>
       <c r="V33" s="7"/>
       <c r="W33" s="7"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X33" s="7"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1612,8 +1658,9 @@
       <c r="U34" s="7"/>
       <c r="V34" s="7"/>
       <c r="W34" s="7"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X34" s="7"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1637,8 +1684,9 @@
       <c r="U35" s="7"/>
       <c r="V35" s="7"/>
       <c r="W35" s="7"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X35" s="7"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1662,8 +1710,9 @@
       <c r="U36" s="7"/>
       <c r="V36" s="7"/>
       <c r="W36" s="7"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X36" s="7"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1687,8 +1736,9 @@
       <c r="U37" s="7"/>
       <c r="V37" s="7"/>
       <c r="W37" s="7"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X37" s="7"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1712,8 +1762,9 @@
       <c r="U38" s="7"/>
       <c r="V38" s="7"/>
       <c r="W38" s="7"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X38" s="7"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1737,8 +1788,9 @@
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>
       <c r="W39" s="7"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X39" s="7"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1762,8 +1814,9 @@
       <c r="U40" s="7"/>
       <c r="V40" s="7"/>
       <c r="W40" s="7"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X40" s="7"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1787,8 +1840,9 @@
       <c r="U41" s="7"/>
       <c r="V41" s="7"/>
       <c r="W41" s="7"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X41" s="7"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1812,8 +1866,9 @@
       <c r="U42" s="7"/>
       <c r="V42" s="7"/>
       <c r="W42" s="7"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X42" s="7"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1837,8 +1892,9 @@
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
       <c r="W43" s="7"/>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X43" s="7"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1862,8 +1918,9 @@
       <c r="U44" s="7"/>
       <c r="V44" s="7"/>
       <c r="W44" s="7"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X44" s="7"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1887,8 +1944,9 @@
       <c r="U45" s="7"/>
       <c r="V45" s="7"/>
       <c r="W45" s="7"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X45" s="7"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1912,8 +1970,9 @@
       <c r="U46" s="7"/>
       <c r="V46" s="7"/>
       <c r="W46" s="7"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X46" s="7"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1937,8 +1996,9 @@
       <c r="U47" s="7"/>
       <c r="V47" s="7"/>
       <c r="W47" s="7"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X47" s="7"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1962,8 +2022,9 @@
       <c r="U48" s="7"/>
       <c r="V48" s="7"/>
       <c r="W48" s="7"/>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X48" s="7"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1987,8 +2048,9 @@
       <c r="U49" s="7"/>
       <c r="V49" s="7"/>
       <c r="W49" s="7"/>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X49" s="7"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -2012,8 +2074,9 @@
       <c r="U50" s="7"/>
       <c r="V50" s="7"/>
       <c r="W50" s="7"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X50" s="7"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -2037,8 +2100,9 @@
       <c r="U51" s="7"/>
       <c r="V51" s="7"/>
       <c r="W51" s="7"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X51" s="7"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -2062,8 +2126,9 @@
       <c r="U52" s="7"/>
       <c r="V52" s="7"/>
       <c r="W52" s="7"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X52" s="7"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -2087,8 +2152,9 @@
       <c r="U53" s="7"/>
       <c r="V53" s="7"/>
       <c r="W53" s="7"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X53" s="7"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -2112,8 +2178,9 @@
       <c r="U54" s="7"/>
       <c r="V54" s="7"/>
       <c r="W54" s="7"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X54" s="7"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -2137,8 +2204,9 @@
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
       <c r="W55" s="7"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X55" s="7"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -2162,8 +2230,9 @@
       <c r="U56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X56" s="7"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -2187,8 +2256,9 @@
       <c r="U57" s="7"/>
       <c r="V57" s="7"/>
       <c r="W57" s="7"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X57" s="7"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -2212,8 +2282,9 @@
       <c r="U58" s="7"/>
       <c r="V58" s="7"/>
       <c r="W58" s="7"/>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X58" s="7"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -2237,8 +2308,9 @@
       <c r="U59" s="7"/>
       <c r="V59" s="7"/>
       <c r="W59" s="7"/>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X59" s="7"/>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -2262,8 +2334,9 @@
       <c r="U60" s="7"/>
       <c r="V60" s="7"/>
       <c r="W60" s="7"/>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X60" s="7"/>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -2287,8 +2360,9 @@
       <c r="U61" s="7"/>
       <c r="V61" s="7"/>
       <c r="W61" s="7"/>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X61" s="7"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -2312,8 +2386,9 @@
       <c r="U62" s="7"/>
       <c r="V62" s="7"/>
       <c r="W62" s="7"/>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X62" s="7"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -2337,8 +2412,9 @@
       <c r="U63" s="7"/>
       <c r="V63" s="7"/>
       <c r="W63" s="7"/>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X63" s="7"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -2362,8 +2438,9 @@
       <c r="U64" s="7"/>
       <c r="V64" s="7"/>
       <c r="W64" s="7"/>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X64" s="7"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -2387,8 +2464,9 @@
       <c r="U65" s="7"/>
       <c r="V65" s="7"/>
       <c r="W65" s="7"/>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X65" s="7"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -2412,8 +2490,9 @@
       <c r="U66" s="7"/>
       <c r="V66" s="7"/>
       <c r="W66" s="7"/>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X66" s="7"/>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -2437,8 +2516,9 @@
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
       <c r="W67" s="7"/>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X67" s="7"/>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -2462,8 +2542,9 @@
       <c r="U68" s="7"/>
       <c r="V68" s="7"/>
       <c r="W68" s="7"/>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X68" s="7"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -2487,8 +2568,9 @@
       <c r="U69" s="7"/>
       <c r="V69" s="7"/>
       <c r="W69" s="7"/>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X69" s="7"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -2512,8 +2594,9 @@
       <c r="U70" s="7"/>
       <c r="V70" s="7"/>
       <c r="W70" s="7"/>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X70" s="7"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -2537,8 +2620,9 @@
       <c r="U71" s="7"/>
       <c r="V71" s="7"/>
       <c r="W71" s="7"/>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X71" s="7"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -2562,8 +2646,9 @@
       <c r="U72" s="7"/>
       <c r="V72" s="7"/>
       <c r="W72" s="7"/>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X72" s="7"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -2587,8 +2672,9 @@
       <c r="U73" s="7"/>
       <c r="V73" s="7"/>
       <c r="W73" s="7"/>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X73" s="7"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -2612,8 +2698,9 @@
       <c r="U74" s="7"/>
       <c r="V74" s="7"/>
       <c r="W74" s="7"/>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X74" s="7"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2637,8 +2724,9 @@
       <c r="U75" s="7"/>
       <c r="V75" s="7"/>
       <c r="W75" s="7"/>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X75" s="7"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -2662,8 +2750,9 @@
       <c r="U76" s="7"/>
       <c r="V76" s="7"/>
       <c r="W76" s="7"/>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X76" s="7"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -2687,8 +2776,9 @@
       <c r="U77" s="7"/>
       <c r="V77" s="7"/>
       <c r="W77" s="7"/>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X77" s="7"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -2712,8 +2802,9 @@
       <c r="U78" s="7"/>
       <c r="V78" s="7"/>
       <c r="W78" s="7"/>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X78" s="7"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -2737,8 +2828,9 @@
       <c r="U79" s="7"/>
       <c r="V79" s="7"/>
       <c r="W79" s="7"/>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X79" s="7"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -2762,8 +2854,9 @@
       <c r="U80" s="7"/>
       <c r="V80" s="7"/>
       <c r="W80" s="7"/>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X80" s="7"/>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -2787,8 +2880,9 @@
       <c r="U81" s="7"/>
       <c r="V81" s="7"/>
       <c r="W81" s="7"/>
-    </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X81" s="7"/>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -2812,8 +2906,9 @@
       <c r="U82" s="7"/>
       <c r="V82" s="7"/>
       <c r="W82" s="7"/>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X82" s="7"/>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -2837,8 +2932,9 @@
       <c r="U83" s="7"/>
       <c r="V83" s="7"/>
       <c r="W83" s="7"/>
-    </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X83" s="7"/>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -2862,8 +2958,9 @@
       <c r="U84" s="7"/>
       <c r="V84" s="7"/>
       <c r="W84" s="7"/>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X84" s="7"/>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -2887,8 +2984,9 @@
       <c r="U85" s="7"/>
       <c r="V85" s="7"/>
       <c r="W85" s="7"/>
-    </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X85" s="7"/>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -2912,8 +3010,9 @@
       <c r="U86" s="7"/>
       <c r="V86" s="7"/>
       <c r="W86" s="7"/>
-    </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X86" s="7"/>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -2937,8 +3036,9 @@
       <c r="U87" s="7"/>
       <c r="V87" s="7"/>
       <c r="W87" s="7"/>
-    </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X87" s="7"/>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -2962,8 +3062,9 @@
       <c r="U88" s="7"/>
       <c r="V88" s="7"/>
       <c r="W88" s="7"/>
-    </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X88" s="7"/>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -2987,8 +3088,9 @@
       <c r="U89" s="7"/>
       <c r="V89" s="7"/>
       <c r="W89" s="7"/>
-    </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X89" s="7"/>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -3012,8 +3114,9 @@
       <c r="U90" s="7"/>
       <c r="V90" s="7"/>
       <c r="W90" s="7"/>
-    </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X90" s="7"/>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -3037,8 +3140,9 @@
       <c r="U91" s="7"/>
       <c r="V91" s="7"/>
       <c r="W91" s="7"/>
-    </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X91" s="7"/>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -3062,8 +3166,9 @@
       <c r="U92" s="7"/>
       <c r="V92" s="7"/>
       <c r="W92" s="7"/>
-    </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X92" s="7"/>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -3087,8 +3192,9 @@
       <c r="U93" s="7"/>
       <c r="V93" s="7"/>
       <c r="W93" s="7"/>
-    </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X93" s="7"/>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -3112,8 +3218,9 @@
       <c r="U94" s="7"/>
       <c r="V94" s="7"/>
       <c r="W94" s="7"/>
-    </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X94" s="7"/>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -3137,8 +3244,9 @@
       <c r="U95" s="7"/>
       <c r="V95" s="7"/>
       <c r="W95" s="7"/>
-    </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X95" s="7"/>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -3162,8 +3270,9 @@
       <c r="U96" s="7"/>
       <c r="V96" s="7"/>
       <c r="W96" s="7"/>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X96" s="7"/>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -3187,8 +3296,9 @@
       <c r="U97" s="7"/>
       <c r="V97" s="7"/>
       <c r="W97" s="7"/>
-    </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X97" s="7"/>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -3212,8 +3322,9 @@
       <c r="U98" s="7"/>
       <c r="V98" s="7"/>
       <c r="W98" s="7"/>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X98" s="7"/>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -3237,8 +3348,9 @@
       <c r="U99" s="7"/>
       <c r="V99" s="7"/>
       <c r="W99" s="7"/>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X99" s="7"/>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -3262,8 +3374,9 @@
       <c r="U100" s="7"/>
       <c r="V100" s="7"/>
       <c r="W100" s="7"/>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X100" s="7"/>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -3287,8 +3400,9 @@
       <c r="U101" s="7"/>
       <c r="V101" s="7"/>
       <c r="W101" s="7"/>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X101" s="7"/>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -3312,8 +3426,9 @@
       <c r="U102" s="7"/>
       <c r="V102" s="7"/>
       <c r="W102" s="7"/>
-    </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X102" s="7"/>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -3337,8 +3452,9 @@
       <c r="U103" s="7"/>
       <c r="V103" s="7"/>
       <c r="W103" s="7"/>
-    </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X103" s="7"/>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -3362,8 +3478,9 @@
       <c r="U104" s="7"/>
       <c r="V104" s="7"/>
       <c r="W104" s="7"/>
-    </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X104" s="7"/>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -3387,8 +3504,9 @@
       <c r="U105" s="7"/>
       <c r="V105" s="7"/>
       <c r="W105" s="7"/>
-    </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X105" s="7"/>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -3412,8 +3530,9 @@
       <c r="U106" s="7"/>
       <c r="V106" s="7"/>
       <c r="W106" s="7"/>
-    </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X106" s="7"/>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -3437,8 +3556,9 @@
       <c r="U107" s="7"/>
       <c r="V107" s="7"/>
       <c r="W107" s="7"/>
-    </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X107" s="7"/>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -3462,8 +3582,9 @@
       <c r="U108" s="7"/>
       <c r="V108" s="7"/>
       <c r="W108" s="7"/>
-    </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X108" s="7"/>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -3487,8 +3608,9 @@
       <c r="U109" s="7"/>
       <c r="V109" s="7"/>
       <c r="W109" s="7"/>
-    </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X109" s="7"/>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -3512,8 +3634,9 @@
       <c r="U110" s="7"/>
       <c r="V110" s="7"/>
       <c r="W110" s="7"/>
-    </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X110" s="7"/>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -3537,8 +3660,9 @@
       <c r="U111" s="7"/>
       <c r="V111" s="7"/>
       <c r="W111" s="7"/>
-    </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X111" s="7"/>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -3562,8 +3686,9 @@
       <c r="U112" s="7"/>
       <c r="V112" s="7"/>
       <c r="W112" s="7"/>
-    </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X112" s="7"/>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -3587,8 +3712,9 @@
       <c r="U113" s="7"/>
       <c r="V113" s="7"/>
       <c r="W113" s="7"/>
-    </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X113" s="7"/>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -3612,8 +3738,9 @@
       <c r="U114" s="7"/>
       <c r="V114" s="7"/>
       <c r="W114" s="7"/>
-    </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X114" s="7"/>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -3637,8 +3764,9 @@
       <c r="U115" s="7"/>
       <c r="V115" s="7"/>
       <c r="W115" s="7"/>
-    </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X115" s="7"/>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -3662,8 +3790,9 @@
       <c r="U116" s="7"/>
       <c r="V116" s="7"/>
       <c r="W116" s="7"/>
-    </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X116" s="7"/>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -3687,8 +3816,9 @@
       <c r="U117" s="7"/>
       <c r="V117" s="7"/>
       <c r="W117" s="7"/>
-    </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X117" s="7"/>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -3712,8 +3842,9 @@
       <c r="U118" s="7"/>
       <c r="V118" s="7"/>
       <c r="W118" s="7"/>
-    </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X118" s="7"/>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -3737,8 +3868,9 @@
       <c r="U119" s="7"/>
       <c r="V119" s="7"/>
       <c r="W119" s="7"/>
-    </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X119" s="7"/>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -3762,8 +3894,9 @@
       <c r="U120" s="7"/>
       <c r="V120" s="7"/>
       <c r="W120" s="7"/>
-    </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X120" s="7"/>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -3787,8 +3920,9 @@
       <c r="U121" s="7"/>
       <c r="V121" s="7"/>
       <c r="W121" s="7"/>
-    </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X121" s="7"/>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -3812,8 +3946,9 @@
       <c r="U122" s="7"/>
       <c r="V122" s="7"/>
       <c r="W122" s="7"/>
-    </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X122" s="7"/>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -3837,8 +3972,9 @@
       <c r="U123" s="7"/>
       <c r="V123" s="7"/>
       <c r="W123" s="7"/>
-    </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X123" s="7"/>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -3862,8 +3998,9 @@
       <c r="U124" s="7"/>
       <c r="V124" s="7"/>
       <c r="W124" s="7"/>
-    </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X124" s="7"/>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
@@ -3887,8 +4024,9 @@
       <c r="U125" s="7"/>
       <c r="V125" s="7"/>
       <c r="W125" s="7"/>
-    </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X125" s="7"/>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
@@ -3912,8 +4050,9 @@
       <c r="U126" s="7"/>
       <c r="V126" s="7"/>
       <c r="W126" s="7"/>
-    </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X126" s="7"/>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
@@ -3937,8 +4076,9 @@
       <c r="U127" s="7"/>
       <c r="V127" s="7"/>
       <c r="W127" s="7"/>
-    </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X127" s="7"/>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -3962,8 +4102,9 @@
       <c r="U128" s="7"/>
       <c r="V128" s="7"/>
       <c r="W128" s="7"/>
-    </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X128" s="7"/>
+    </row>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
@@ -3987,8 +4128,9 @@
       <c r="U129" s="7"/>
       <c r="V129" s="7"/>
       <c r="W129" s="7"/>
-    </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X129" s="7"/>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -4012,8 +4154,9 @@
       <c r="U130" s="7"/>
       <c r="V130" s="7"/>
       <c r="W130" s="7"/>
-    </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X130" s="7"/>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -4037,8 +4180,9 @@
       <c r="U131" s="7"/>
       <c r="V131" s="7"/>
       <c r="W131" s="7"/>
-    </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X131" s="7"/>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
@@ -4062,8 +4206,9 @@
       <c r="U132" s="7"/>
       <c r="V132" s="7"/>
       <c r="W132" s="7"/>
-    </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X132" s="7"/>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
@@ -4087,8 +4232,9 @@
       <c r="U133" s="7"/>
       <c r="V133" s="7"/>
       <c r="W133" s="7"/>
-    </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X133" s="7"/>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -4112,8 +4258,9 @@
       <c r="U134" s="7"/>
       <c r="V134" s="7"/>
       <c r="W134" s="7"/>
-    </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X134" s="7"/>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -4137,8 +4284,9 @@
       <c r="U135" s="7"/>
       <c r="V135" s="7"/>
       <c r="W135" s="7"/>
-    </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X135" s="7"/>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -4162,8 +4310,9 @@
       <c r="U136" s="7"/>
       <c r="V136" s="7"/>
       <c r="W136" s="7"/>
-    </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X136" s="7"/>
+    </row>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -4187,8 +4336,9 @@
       <c r="U137" s="7"/>
       <c r="V137" s="7"/>
       <c r="W137" s="7"/>
-    </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X137" s="7"/>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
@@ -4212,8 +4362,9 @@
       <c r="U138" s="7"/>
       <c r="V138" s="7"/>
       <c r="W138" s="7"/>
-    </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X138" s="7"/>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
@@ -4237,8 +4388,9 @@
       <c r="U139" s="7"/>
       <c r="V139" s="7"/>
       <c r="W139" s="7"/>
-    </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X139" s="7"/>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
@@ -4262,8 +4414,9 @@
       <c r="U140" s="7"/>
       <c r="V140" s="7"/>
       <c r="W140" s="7"/>
-    </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X140" s="7"/>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
@@ -4287,8 +4440,9 @@
       <c r="U141" s="7"/>
       <c r="V141" s="7"/>
       <c r="W141" s="7"/>
-    </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X141" s="7"/>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
@@ -4312,8 +4466,9 @@
       <c r="U142" s="7"/>
       <c r="V142" s="7"/>
       <c r="W142" s="7"/>
-    </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X142" s="7"/>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
@@ -4337,8 +4492,9 @@
       <c r="U143" s="7"/>
       <c r="V143" s="7"/>
       <c r="W143" s="7"/>
-    </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X143" s="7"/>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
@@ -4362,8 +4518,9 @@
       <c r="U144" s="7"/>
       <c r="V144" s="7"/>
       <c r="W144" s="7"/>
-    </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X144" s="7"/>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
@@ -4387,8 +4544,9 @@
       <c r="U145" s="7"/>
       <c r="V145" s="7"/>
       <c r="W145" s="7"/>
-    </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X145" s="7"/>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
@@ -4412,8 +4570,9 @@
       <c r="U146" s="7"/>
       <c r="V146" s="7"/>
       <c r="W146" s="7"/>
-    </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X146" s="7"/>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -4437,8 +4596,9 @@
       <c r="U147" s="7"/>
       <c r="V147" s="7"/>
       <c r="W147" s="7"/>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X147" s="7"/>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
@@ -4462,8 +4622,9 @@
       <c r="U148" s="7"/>
       <c r="V148" s="7"/>
       <c r="W148" s="7"/>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X148" s="7"/>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
@@ -4487,8 +4648,9 @@
       <c r="U149" s="7"/>
       <c r="V149" s="7"/>
       <c r="W149" s="7"/>
-    </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X149" s="7"/>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
@@ -4512,8 +4674,9 @@
       <c r="U150" s="7"/>
       <c r="V150" s="7"/>
       <c r="W150" s="7"/>
-    </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X150" s="7"/>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
@@ -4537,8 +4700,9 @@
       <c r="U151" s="7"/>
       <c r="V151" s="7"/>
       <c r="W151" s="7"/>
-    </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X151" s="7"/>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
@@ -4562,8 +4726,9 @@
       <c r="U152" s="7"/>
       <c r="V152" s="7"/>
       <c r="W152" s="7"/>
-    </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X152" s="7"/>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
@@ -4587,8 +4752,9 @@
       <c r="U153" s="7"/>
       <c r="V153" s="7"/>
       <c r="W153" s="7"/>
-    </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X153" s="7"/>
+    </row>
+    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
@@ -4612,8 +4778,9 @@
       <c r="U154" s="7"/>
       <c r="V154" s="7"/>
       <c r="W154" s="7"/>
-    </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X154" s="7"/>
+    </row>
+    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
@@ -4637,8 +4804,9 @@
       <c r="U155" s="7"/>
       <c r="V155" s="7"/>
       <c r="W155" s="7"/>
-    </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X155" s="7"/>
+    </row>
+    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
@@ -4662,8 +4830,9 @@
       <c r="U156" s="7"/>
       <c r="V156" s="7"/>
       <c r="W156" s="7"/>
-    </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X156" s="7"/>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -4687,8 +4856,9 @@
       <c r="U157" s="7"/>
       <c r="V157" s="7"/>
       <c r="W157" s="7"/>
-    </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X157" s="7"/>
+    </row>
+    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
@@ -4712,8 +4882,9 @@
       <c r="U158" s="7"/>
       <c r="V158" s="7"/>
       <c r="W158" s="7"/>
-    </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X158" s="7"/>
+    </row>
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
@@ -4737,8 +4908,9 @@
       <c r="U159" s="7"/>
       <c r="V159" s="7"/>
       <c r="W159" s="7"/>
-    </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X159" s="7"/>
+    </row>
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
@@ -4762,8 +4934,9 @@
       <c r="U160" s="7"/>
       <c r="V160" s="7"/>
       <c r="W160" s="7"/>
-    </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X160" s="7"/>
+    </row>
+    <row r="161" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
@@ -4787,8 +4960,9 @@
       <c r="U161" s="7"/>
       <c r="V161" s="7"/>
       <c r="W161" s="7"/>
-    </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X161" s="7"/>
+    </row>
+    <row r="162" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -4812,8 +4986,9 @@
       <c r="U162" s="7"/>
       <c r="V162" s="7"/>
       <c r="W162" s="7"/>
-    </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X162" s="7"/>
+    </row>
+    <row r="163" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -4837,8 +5012,9 @@
       <c r="U163" s="7"/>
       <c r="V163" s="7"/>
       <c r="W163" s="7"/>
-    </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X163" s="7"/>
+    </row>
+    <row r="164" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -4862,8 +5038,9 @@
       <c r="U164" s="7"/>
       <c r="V164" s="7"/>
       <c r="W164" s="7"/>
-    </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X164" s="7"/>
+    </row>
+    <row r="165" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
@@ -4887,8 +5064,9 @@
       <c r="U165" s="7"/>
       <c r="V165" s="7"/>
       <c r="W165" s="7"/>
-    </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X165" s="7"/>
+    </row>
+    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -4912,8 +5090,9 @@
       <c r="U166" s="7"/>
       <c r="V166" s="7"/>
       <c r="W166" s="7"/>
-    </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X166" s="7"/>
+    </row>
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -4937,8 +5116,9 @@
       <c r="U167" s="7"/>
       <c r="V167" s="7"/>
       <c r="W167" s="7"/>
-    </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X167" s="7"/>
+    </row>
+    <row r="168" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -4962,8 +5142,9 @@
       <c r="U168" s="7"/>
       <c r="V168" s="7"/>
       <c r="W168" s="7"/>
-    </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X168" s="7"/>
+    </row>
+    <row r="169" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -4987,8 +5168,9 @@
       <c r="U169" s="7"/>
       <c r="V169" s="7"/>
       <c r="W169" s="7"/>
-    </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X169" s="7"/>
+    </row>
+    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -5012,8 +5194,9 @@
       <c r="U170" s="7"/>
       <c r="V170" s="7"/>
       <c r="W170" s="7"/>
-    </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X170" s="7"/>
+    </row>
+    <row r="171" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
@@ -5037,8 +5220,9 @@
       <c r="U171" s="7"/>
       <c r="V171" s="7"/>
       <c r="W171" s="7"/>
-    </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X171" s="7"/>
+    </row>
+    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -5062,8 +5246,9 @@
       <c r="U172" s="7"/>
       <c r="V172" s="7"/>
       <c r="W172" s="7"/>
-    </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X172" s="7"/>
+    </row>
+    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -5087,8 +5272,9 @@
       <c r="U173" s="7"/>
       <c r="V173" s="7"/>
       <c r="W173" s="7"/>
-    </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X173" s="7"/>
+    </row>
+    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
@@ -5112,8 +5298,9 @@
       <c r="U174" s="7"/>
       <c r="V174" s="7"/>
       <c r="W174" s="7"/>
-    </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X174" s="7"/>
+    </row>
+    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
@@ -5137,8 +5324,9 @@
       <c r="U175" s="7"/>
       <c r="V175" s="7"/>
       <c r="W175" s="7"/>
-    </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X175" s="7"/>
+    </row>
+    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -5162,8 +5350,9 @@
       <c r="U176" s="7"/>
       <c r="V176" s="7"/>
       <c r="W176" s="7"/>
-    </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X176" s="7"/>
+    </row>
+    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -5187,8 +5376,9 @@
       <c r="U177" s="7"/>
       <c r="V177" s="7"/>
       <c r="W177" s="7"/>
-    </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X177" s="7"/>
+    </row>
+    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -5212,8 +5402,9 @@
       <c r="U178" s="7"/>
       <c r="V178" s="7"/>
       <c r="W178" s="7"/>
-    </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X178" s="7"/>
+    </row>
+    <row r="179" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -5237,8 +5428,9 @@
       <c r="U179" s="7"/>
       <c r="V179" s="7"/>
       <c r="W179" s="7"/>
-    </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X179" s="7"/>
+    </row>
+    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -5262,8 +5454,9 @@
       <c r="U180" s="7"/>
       <c r="V180" s="7"/>
       <c r="W180" s="7"/>
-    </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X180" s="7"/>
+    </row>
+    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -5287,8 +5480,9 @@
       <c r="U181" s="7"/>
       <c r="V181" s="7"/>
       <c r="W181" s="7"/>
-    </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X181" s="7"/>
+    </row>
+    <row r="182" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
@@ -5312,8 +5506,9 @@
       <c r="U182" s="7"/>
       <c r="V182" s="7"/>
       <c r="W182" s="7"/>
-    </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X182" s="7"/>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
@@ -5337,8 +5532,9 @@
       <c r="U183" s="7"/>
       <c r="V183" s="7"/>
       <c r="W183" s="7"/>
-    </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X183" s="7"/>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
@@ -5362,8 +5558,9 @@
       <c r="U184" s="7"/>
       <c r="V184" s="7"/>
       <c r="W184" s="7"/>
-    </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X184" s="7"/>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
@@ -5387,8 +5584,9 @@
       <c r="U185" s="7"/>
       <c r="V185" s="7"/>
       <c r="W185" s="7"/>
-    </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X185" s="7"/>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
@@ -5412,8 +5610,9 @@
       <c r="U186" s="7"/>
       <c r="V186" s="7"/>
       <c r="W186" s="7"/>
-    </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X186" s="7"/>
+    </row>
+    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
@@ -5437,8 +5636,9 @@
       <c r="U187" s="7"/>
       <c r="V187" s="7"/>
       <c r="W187" s="7"/>
-    </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X187" s="7"/>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
@@ -5462,8 +5662,9 @@
       <c r="U188" s="7"/>
       <c r="V188" s="7"/>
       <c r="W188" s="7"/>
-    </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X188" s="7"/>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
@@ -5487,8 +5688,9 @@
       <c r="U189" s="7"/>
       <c r="V189" s="7"/>
       <c r="W189" s="7"/>
-    </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X189" s="7"/>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
@@ -5512,8 +5714,9 @@
       <c r="U190" s="7"/>
       <c r="V190" s="7"/>
       <c r="W190" s="7"/>
-    </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X190" s="7"/>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
@@ -5537,8 +5740,9 @@
       <c r="U191" s="7"/>
       <c r="V191" s="7"/>
       <c r="W191" s="7"/>
-    </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X191" s="7"/>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -5562,8 +5766,9 @@
       <c r="U192" s="7"/>
       <c r="V192" s="7"/>
       <c r="W192" s="7"/>
-    </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X192" s="7"/>
+    </row>
+    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A193" s="7"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
@@ -5587,8 +5792,9 @@
       <c r="U193" s="7"/>
       <c r="V193" s="7"/>
       <c r="W193" s="7"/>
-    </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X193" s="7"/>
+    </row>
+    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A194" s="7"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
@@ -5612,8 +5818,9 @@
       <c r="U194" s="7"/>
       <c r="V194" s="7"/>
       <c r="W194" s="7"/>
-    </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X194" s="7"/>
+    </row>
+    <row r="195" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A195" s="7"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
@@ -5637,8 +5844,9 @@
       <c r="U195" s="7"/>
       <c r="V195" s="7"/>
       <c r="W195" s="7"/>
-    </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X195" s="7"/>
+    </row>
+    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A196" s="7"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
@@ -5662,8 +5870,9 @@
       <c r="U196" s="7"/>
       <c r="V196" s="7"/>
       <c r="W196" s="7"/>
-    </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X196" s="7"/>
+    </row>
+    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A197" s="7"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
@@ -5687,8 +5896,9 @@
       <c r="U197" s="7"/>
       <c r="V197" s="7"/>
       <c r="W197" s="7"/>
-    </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X197" s="7"/>
+    </row>
+    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A198" s="7"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
@@ -5712,8 +5922,9 @@
       <c r="U198" s="7"/>
       <c r="V198" s="7"/>
       <c r="W198" s="7"/>
-    </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X198" s="7"/>
+    </row>
+    <row r="199" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A199" s="7"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
@@ -5737,8 +5948,9 @@
       <c r="U199" s="7"/>
       <c r="V199" s="7"/>
       <c r="W199" s="7"/>
-    </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X199" s="7"/>
+    </row>
+    <row r="200" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A200" s="7"/>
       <c r="B200" s="7"/>
       <c r="C200" s="7"/>
@@ -5762,8 +5974,9 @@
       <c r="U200" s="7"/>
       <c r="V200" s="7"/>
       <c r="W200" s="7"/>
-    </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X200" s="7"/>
+    </row>
+    <row r="201" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A201" s="7"/>
       <c r="B201" s="7"/>
       <c r="C201" s="7"/>
@@ -5787,8 +6000,9 @@
       <c r="U201" s="7"/>
       <c r="V201" s="7"/>
       <c r="W201" s="7"/>
-    </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X201" s="7"/>
+    </row>
+    <row r="202" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A202" s="7"/>
       <c r="B202" s="7"/>
       <c r="C202" s="7"/>
@@ -5812,8 +6026,9 @@
       <c r="U202" s="7"/>
       <c r="V202" s="7"/>
       <c r="W202" s="7"/>
-    </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X202" s="7"/>
+    </row>
+    <row r="203" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A203" s="7"/>
       <c r="B203" s="7"/>
       <c r="C203" s="7"/>
@@ -5837,8 +6052,9 @@
       <c r="U203" s="7"/>
       <c r="V203" s="7"/>
       <c r="W203" s="7"/>
-    </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X203" s="7"/>
+    </row>
+    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A204" s="7"/>
       <c r="B204" s="7"/>
       <c r="C204" s="7"/>
@@ -5862,8 +6078,9 @@
       <c r="U204" s="7"/>
       <c r="V204" s="7"/>
       <c r="W204" s="7"/>
-    </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X204" s="7"/>
+    </row>
+    <row r="205" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A205" s="7"/>
       <c r="B205" s="7"/>
       <c r="C205" s="7"/>
@@ -5887,8 +6104,9 @@
       <c r="U205" s="7"/>
       <c r="V205" s="7"/>
       <c r="W205" s="7"/>
-    </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X205" s="7"/>
+    </row>
+    <row r="206" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A206" s="7"/>
       <c r="B206" s="7"/>
       <c r="C206" s="7"/>
@@ -5912,8 +6130,9 @@
       <c r="U206" s="7"/>
       <c r="V206" s="7"/>
       <c r="W206" s="7"/>
-    </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X206" s="7"/>
+    </row>
+    <row r="207" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A207" s="7"/>
       <c r="B207" s="7"/>
       <c r="C207" s="7"/>
@@ -5937,8 +6156,9 @@
       <c r="U207" s="7"/>
       <c r="V207" s="7"/>
       <c r="W207" s="7"/>
-    </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X207" s="7"/>
+    </row>
+    <row r="208" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A208" s="7"/>
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
@@ -5962,8 +6182,9 @@
       <c r="U208" s="7"/>
       <c r="V208" s="7"/>
       <c r="W208" s="7"/>
-    </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X208" s="7"/>
+    </row>
+    <row r="209" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A209" s="7"/>
       <c r="B209" s="7"/>
       <c r="C209" s="7"/>
@@ -5987,8 +6208,9 @@
       <c r="U209" s="7"/>
       <c r="V209" s="7"/>
       <c r="W209" s="7"/>
-    </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X209" s="7"/>
+    </row>
+    <row r="210" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A210" s="7"/>
       <c r="B210" s="7"/>
       <c r="C210" s="7"/>
@@ -6012,8 +6234,9 @@
       <c r="U210" s="7"/>
       <c r="V210" s="7"/>
       <c r="W210" s="7"/>
-    </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X210" s="7"/>
+    </row>
+    <row r="211" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A211" s="7"/>
       <c r="B211" s="7"/>
       <c r="C211" s="7"/>
@@ -6037,8 +6260,9 @@
       <c r="U211" s="7"/>
       <c r="V211" s="7"/>
       <c r="W211" s="7"/>
-    </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X211" s="7"/>
+    </row>
+    <row r="212" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A212" s="7"/>
       <c r="B212" s="7"/>
       <c r="C212" s="7"/>
@@ -6062,8 +6286,9 @@
       <c r="U212" s="7"/>
       <c r="V212" s="7"/>
       <c r="W212" s="7"/>
-    </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X212" s="7"/>
+    </row>
+    <row r="213" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A213" s="7"/>
       <c r="B213" s="7"/>
       <c r="C213" s="7"/>
@@ -6087,8 +6312,9 @@
       <c r="U213" s="7"/>
       <c r="V213" s="7"/>
       <c r="W213" s="7"/>
-    </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X213" s="7"/>
+    </row>
+    <row r="214" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A214" s="7"/>
       <c r="B214" s="7"/>
       <c r="C214" s="7"/>
@@ -6112,8 +6338,9 @@
       <c r="U214" s="7"/>
       <c r="V214" s="7"/>
       <c r="W214" s="7"/>
-    </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X214" s="7"/>
+    </row>
+    <row r="215" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A215" s="7"/>
       <c r="B215" s="7"/>
       <c r="C215" s="7"/>
@@ -6137,8 +6364,9 @@
       <c r="U215" s="7"/>
       <c r="V215" s="7"/>
       <c r="W215" s="7"/>
-    </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X215" s="7"/>
+    </row>
+    <row r="216" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A216" s="7"/>
       <c r="B216" s="7"/>
       <c r="C216" s="7"/>
@@ -6162,8 +6390,9 @@
       <c r="U216" s="7"/>
       <c r="V216" s="7"/>
       <c r="W216" s="7"/>
-    </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X216" s="7"/>
+    </row>
+    <row r="217" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A217" s="7"/>
       <c r="B217" s="7"/>
       <c r="C217" s="7"/>
@@ -6187,8 +6416,9 @@
       <c r="U217" s="7"/>
       <c r="V217" s="7"/>
       <c r="W217" s="7"/>
-    </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X217" s="7"/>
+    </row>
+    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A218" s="7"/>
       <c r="B218" s="7"/>
       <c r="C218" s="7"/>
@@ -6212,8 +6442,9 @@
       <c r="U218" s="7"/>
       <c r="V218" s="7"/>
       <c r="W218" s="7"/>
-    </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X218" s="7"/>
+    </row>
+    <row r="219" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A219" s="7"/>
       <c r="B219" s="7"/>
       <c r="C219" s="7"/>
@@ -6237,8 +6468,9 @@
       <c r="U219" s="7"/>
       <c r="V219" s="7"/>
       <c r="W219" s="7"/>
-    </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X219" s="7"/>
+    </row>
+    <row r="220" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A220" s="7"/>
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
@@ -6262,8 +6494,9 @@
       <c r="U220" s="7"/>
       <c r="V220" s="7"/>
       <c r="W220" s="7"/>
-    </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X220" s="7"/>
+    </row>
+    <row r="221" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A221" s="7"/>
       <c r="B221" s="7"/>
       <c r="C221" s="7"/>
@@ -6287,8 +6520,9 @@
       <c r="U221" s="7"/>
       <c r="V221" s="7"/>
       <c r="W221" s="7"/>
-    </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X221" s="7"/>
+    </row>
+    <row r="222" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A222" s="7"/>
       <c r="B222" s="7"/>
       <c r="C222" s="7"/>
@@ -6312,8 +6546,9 @@
       <c r="U222" s="7"/>
       <c r="V222" s="7"/>
       <c r="W222" s="7"/>
-    </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X222" s="7"/>
+    </row>
+    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A223" s="7"/>
       <c r="B223" s="7"/>
       <c r="C223" s="7"/>
@@ -6337,8 +6572,9 @@
       <c r="U223" s="7"/>
       <c r="V223" s="7"/>
       <c r="W223" s="7"/>
-    </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X223" s="7"/>
+    </row>
+    <row r="224" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A224" s="7"/>
       <c r="B224" s="7"/>
       <c r="C224" s="7"/>
@@ -6362,8 +6598,9 @@
       <c r="U224" s="7"/>
       <c r="V224" s="7"/>
       <c r="W224" s="7"/>
-    </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X224" s="7"/>
+    </row>
+    <row r="225" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A225" s="7"/>
       <c r="B225" s="7"/>
       <c r="C225" s="7"/>
@@ -6387,8 +6624,9 @@
       <c r="U225" s="7"/>
       <c r="V225" s="7"/>
       <c r="W225" s="7"/>
-    </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X225" s="7"/>
+    </row>
+    <row r="226" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A226" s="7"/>
       <c r="B226" s="7"/>
       <c r="C226" s="7"/>
@@ -6412,8 +6650,9 @@
       <c r="U226" s="7"/>
       <c r="V226" s="7"/>
       <c r="W226" s="7"/>
-    </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X226" s="7"/>
+    </row>
+    <row r="227" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A227" s="7"/>
       <c r="B227" s="7"/>
       <c r="C227" s="7"/>
@@ -6437,8 +6676,9 @@
       <c r="U227" s="7"/>
       <c r="V227" s="7"/>
       <c r="W227" s="7"/>
-    </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X227" s="7"/>
+    </row>
+    <row r="228" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A228" s="7"/>
       <c r="B228" s="7"/>
       <c r="C228" s="7"/>
@@ -6462,8 +6702,9 @@
       <c r="U228" s="7"/>
       <c r="V228" s="7"/>
       <c r="W228" s="7"/>
-    </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X228" s="7"/>
+    </row>
+    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A229" s="7"/>
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
@@ -6487,8 +6728,9 @@
       <c r="U229" s="7"/>
       <c r="V229" s="7"/>
       <c r="W229" s="7"/>
-    </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X229" s="7"/>
+    </row>
+    <row r="230" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A230" s="7"/>
       <c r="B230" s="7"/>
       <c r="C230" s="7"/>
@@ -6512,8 +6754,9 @@
       <c r="U230" s="7"/>
       <c r="V230" s="7"/>
       <c r="W230" s="7"/>
-    </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X230" s="7"/>
+    </row>
+    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A231" s="7"/>
       <c r="B231" s="7"/>
       <c r="C231" s="7"/>
@@ -6537,8 +6780,9 @@
       <c r="U231" s="7"/>
       <c r="V231" s="7"/>
       <c r="W231" s="7"/>
-    </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X231" s="7"/>
+    </row>
+    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A232" s="7"/>
       <c r="B232" s="7"/>
       <c r="C232" s="7"/>
@@ -6562,8 +6806,9 @@
       <c r="U232" s="7"/>
       <c r="V232" s="7"/>
       <c r="W232" s="7"/>
-    </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X232" s="7"/>
+    </row>
+    <row r="233" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A233" s="7"/>
       <c r="B233" s="7"/>
       <c r="C233" s="7"/>
@@ -6587,8 +6832,9 @@
       <c r="U233" s="7"/>
       <c r="V233" s="7"/>
       <c r="W233" s="7"/>
-    </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X233" s="7"/>
+    </row>
+    <row r="234" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A234" s="7"/>
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
@@ -6612,8 +6858,9 @@
       <c r="U234" s="7"/>
       <c r="V234" s="7"/>
       <c r="W234" s="7"/>
-    </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X234" s="7"/>
+    </row>
+    <row r="235" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A235" s="7"/>
       <c r="B235" s="7"/>
       <c r="C235" s="7"/>
@@ -6637,8 +6884,9 @@
       <c r="U235" s="7"/>
       <c r="V235" s="7"/>
       <c r="W235" s="7"/>
-    </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X235" s="7"/>
+    </row>
+    <row r="236" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A236" s="7"/>
       <c r="B236" s="7"/>
       <c r="C236" s="7"/>
@@ -6662,8 +6910,9 @@
       <c r="U236" s="7"/>
       <c r="V236" s="7"/>
       <c r="W236" s="7"/>
-    </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X236" s="7"/>
+    </row>
+    <row r="237" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A237" s="7"/>
       <c r="B237" s="7"/>
       <c r="C237" s="7"/>
@@ -6687,8 +6936,9 @@
       <c r="U237" s="7"/>
       <c r="V237" s="7"/>
       <c r="W237" s="7"/>
-    </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X237" s="7"/>
+    </row>
+    <row r="238" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A238" s="7"/>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
@@ -6712,8 +6962,9 @@
       <c r="U238" s="7"/>
       <c r="V238" s="7"/>
       <c r="W238" s="7"/>
-    </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X238" s="7"/>
+    </row>
+    <row r="239" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A239" s="7"/>
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
@@ -6737,8 +6988,9 @@
       <c r="U239" s="7"/>
       <c r="V239" s="7"/>
       <c r="W239" s="7"/>
-    </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X239" s="7"/>
+    </row>
+    <row r="240" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A240" s="7"/>
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>
@@ -6762,8 +7014,9 @@
       <c r="U240" s="7"/>
       <c r="V240" s="7"/>
       <c r="W240" s="7"/>
-    </row>
-    <row r="241" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X240" s="7"/>
+    </row>
+    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A241" s="7"/>
       <c r="B241" s="7"/>
       <c r="C241" s="7"/>
@@ -6787,8 +7040,9 @@
       <c r="U241" s="7"/>
       <c r="V241" s="7"/>
       <c r="W241" s="7"/>
-    </row>
-    <row r="242" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X241" s="7"/>
+    </row>
+    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A242" s="7"/>
       <c r="B242" s="7"/>
       <c r="C242" s="7"/>
@@ -6812,8 +7066,9 @@
       <c r="U242" s="7"/>
       <c r="V242" s="7"/>
       <c r="W242" s="7"/>
-    </row>
-    <row r="243" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X242" s="7"/>
+    </row>
+    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A243" s="7"/>
       <c r="B243" s="7"/>
       <c r="C243" s="7"/>
@@ -6837,8 +7092,9 @@
       <c r="U243" s="7"/>
       <c r="V243" s="7"/>
       <c r="W243" s="7"/>
-    </row>
-    <row r="244" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X243" s="7"/>
+    </row>
+    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A244" s="7"/>
       <c r="B244" s="7"/>
       <c r="C244" s="7"/>
@@ -6862,8 +7118,9 @@
       <c r="U244" s="7"/>
       <c r="V244" s="7"/>
       <c r="W244" s="7"/>
-    </row>
-    <row r="245" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X244" s="7"/>
+    </row>
+    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A245" s="7"/>
       <c r="B245" s="7"/>
       <c r="C245" s="7"/>
@@ -6887,8 +7144,9 @@
       <c r="U245" s="7"/>
       <c r="V245" s="7"/>
       <c r="W245" s="7"/>
-    </row>
-    <row r="246" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X245" s="7"/>
+    </row>
+    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A246" s="7"/>
       <c r="B246" s="7"/>
       <c r="C246" s="7"/>
@@ -6912,8 +7170,9 @@
       <c r="U246" s="7"/>
       <c r="V246" s="7"/>
       <c r="W246" s="7"/>
-    </row>
-    <row r="247" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X246" s="7"/>
+    </row>
+    <row r="247" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A247" s="7"/>
       <c r="B247" s="7"/>
       <c r="C247" s="7"/>
@@ -6937,8 +7196,9 @@
       <c r="U247" s="7"/>
       <c r="V247" s="7"/>
       <c r="W247" s="7"/>
-    </row>
-    <row r="248" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X247" s="7"/>
+    </row>
+    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A248" s="7"/>
       <c r="B248" s="7"/>
       <c r="C248" s="7"/>
@@ -6962,8 +7222,9 @@
       <c r="U248" s="7"/>
       <c r="V248" s="7"/>
       <c r="W248" s="7"/>
-    </row>
-    <row r="249" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X248" s="7"/>
+    </row>
+    <row r="249" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A249" s="7"/>
       <c r="B249" s="7"/>
       <c r="C249" s="7"/>
@@ -6987,8 +7248,9 @@
       <c r="U249" s="7"/>
       <c r="V249" s="7"/>
       <c r="W249" s="7"/>
-    </row>
-    <row r="250" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X249" s="7"/>
+    </row>
+    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A250" s="7"/>
       <c r="B250" s="7"/>
       <c r="C250" s="7"/>
@@ -7012,8 +7274,9 @@
       <c r="U250" s="7"/>
       <c r="V250" s="7"/>
       <c r="W250" s="7"/>
-    </row>
-    <row r="251" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X250" s="7"/>
+    </row>
+    <row r="251" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A251" s="7"/>
       <c r="B251" s="7"/>
       <c r="C251" s="7"/>
@@ -7037,8 +7300,9 @@
       <c r="U251" s="7"/>
       <c r="V251" s="7"/>
       <c r="W251" s="7"/>
-    </row>
-    <row r="252" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X251" s="7"/>
+    </row>
+    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A252" s="7"/>
       <c r="B252" s="7"/>
       <c r="C252" s="7"/>
@@ -7062,8 +7326,9 @@
       <c r="U252" s="7"/>
       <c r="V252" s="7"/>
       <c r="W252" s="7"/>
-    </row>
-    <row r="253" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X252" s="7"/>
+    </row>
+    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A253" s="7"/>
       <c r="B253" s="7"/>
       <c r="C253" s="7"/>
@@ -7087,8 +7352,9 @@
       <c r="U253" s="7"/>
       <c r="V253" s="7"/>
       <c r="W253" s="7"/>
-    </row>
-    <row r="254" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X253" s="7"/>
+    </row>
+    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A254" s="7"/>
       <c r="B254" s="7"/>
       <c r="C254" s="7"/>
@@ -7112,8 +7378,9 @@
       <c r="U254" s="7"/>
       <c r="V254" s="7"/>
       <c r="W254" s="7"/>
-    </row>
-    <row r="255" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X254" s="7"/>
+    </row>
+    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A255" s="7"/>
       <c r="B255" s="7"/>
       <c r="C255" s="7"/>
@@ -7137,8 +7404,9 @@
       <c r="U255" s="7"/>
       <c r="V255" s="7"/>
       <c r="W255" s="7"/>
-    </row>
-    <row r="256" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X255" s="7"/>
+    </row>
+    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A256" s="7"/>
       <c r="B256" s="7"/>
       <c r="C256" s="7"/>
@@ -7162,8 +7430,9 @@
       <c r="U256" s="7"/>
       <c r="V256" s="7"/>
       <c r="W256" s="7"/>
-    </row>
-    <row r="257" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X256" s="7"/>
+    </row>
+    <row r="257" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A257" s="7"/>
       <c r="B257" s="7"/>
       <c r="C257" s="7"/>
@@ -7187,8 +7456,9 @@
       <c r="U257" s="7"/>
       <c r="V257" s="7"/>
       <c r="W257" s="7"/>
-    </row>
-    <row r="258" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X257" s="7"/>
+    </row>
+    <row r="258" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A258" s="7"/>
       <c r="B258" s="7"/>
       <c r="C258" s="7"/>
@@ -7212,8 +7482,9 @@
       <c r="U258" s="7"/>
       <c r="V258" s="7"/>
       <c r="W258" s="7"/>
-    </row>
-    <row r="259" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X258" s="7"/>
+    </row>
+    <row r="259" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A259" s="7"/>
       <c r="B259" s="7"/>
       <c r="C259" s="7"/>
@@ -7237,8 +7508,9 @@
       <c r="U259" s="7"/>
       <c r="V259" s="7"/>
       <c r="W259" s="7"/>
-    </row>
-    <row r="260" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X259" s="7"/>
+    </row>
+    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A260" s="7"/>
       <c r="B260" s="7"/>
       <c r="C260" s="7"/>
@@ -7262,8 +7534,9 @@
       <c r="U260" s="7"/>
       <c r="V260" s="7"/>
       <c r="W260" s="7"/>
-    </row>
-    <row r="261" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X260" s="7"/>
+    </row>
+    <row r="261" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A261" s="7"/>
       <c r="B261" s="7"/>
       <c r="C261" s="7"/>
@@ -7287,8 +7560,9 @@
       <c r="U261" s="7"/>
       <c r="V261" s="7"/>
       <c r="W261" s="7"/>
-    </row>
-    <row r="262" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X261" s="7"/>
+    </row>
+    <row r="262" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A262" s="7"/>
       <c r="B262" s="7"/>
       <c r="C262" s="7"/>
@@ -7312,8 +7586,9 @@
       <c r="U262" s="7"/>
       <c r="V262" s="7"/>
       <c r="W262" s="7"/>
-    </row>
-    <row r="263" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X262" s="7"/>
+    </row>
+    <row r="263" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A263" s="7"/>
       <c r="B263" s="7"/>
       <c r="C263" s="7"/>
@@ -7337,8 +7612,9 @@
       <c r="U263" s="7"/>
       <c r="V263" s="7"/>
       <c r="W263" s="7"/>
-    </row>
-    <row r="264" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X263" s="7"/>
+    </row>
+    <row r="264" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A264" s="7"/>
       <c r="B264" s="7"/>
       <c r="C264" s="7"/>
@@ -7362,8 +7638,9 @@
       <c r="U264" s="7"/>
       <c r="V264" s="7"/>
       <c r="W264" s="7"/>
-    </row>
-    <row r="265" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X264" s="7"/>
+    </row>
+    <row r="265" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A265" s="7"/>
       <c r="B265" s="7"/>
       <c r="C265" s="7"/>
@@ -7387,8 +7664,9 @@
       <c r="U265" s="7"/>
       <c r="V265" s="7"/>
       <c r="W265" s="7"/>
-    </row>
-    <row r="266" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X265" s="7"/>
+    </row>
+    <row r="266" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A266" s="7"/>
       <c r="B266" s="7"/>
       <c r="C266" s="7"/>
@@ -7412,8 +7690,9 @@
       <c r="U266" s="7"/>
       <c r="V266" s="7"/>
       <c r="W266" s="7"/>
-    </row>
-    <row r="267" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X266" s="7"/>
+    </row>
+    <row r="267" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A267" s="7"/>
       <c r="B267" s="7"/>
       <c r="C267" s="7"/>
@@ -7437,8 +7716,9 @@
       <c r="U267" s="7"/>
       <c r="V267" s="7"/>
       <c r="W267" s="7"/>
-    </row>
-    <row r="268" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X267" s="7"/>
+    </row>
+    <row r="268" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A268" s="7"/>
       <c r="B268" s="7"/>
       <c r="C268" s="7"/>
@@ -7462,8 +7742,9 @@
       <c r="U268" s="7"/>
       <c r="V268" s="7"/>
       <c r="W268" s="7"/>
-    </row>
-    <row r="269" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X268" s="7"/>
+    </row>
+    <row r="269" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A269" s="7"/>
       <c r="B269" s="7"/>
       <c r="C269" s="7"/>
@@ -7487,8 +7768,9 @@
       <c r="U269" s="7"/>
       <c r="V269" s="7"/>
       <c r="W269" s="7"/>
-    </row>
-    <row r="270" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X269" s="7"/>
+    </row>
+    <row r="270" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A270" s="7"/>
       <c r="B270" s="7"/>
       <c r="C270" s="7"/>
@@ -7512,8 +7794,9 @@
       <c r="U270" s="7"/>
       <c r="V270" s="7"/>
       <c r="W270" s="7"/>
-    </row>
-    <row r="271" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X270" s="7"/>
+    </row>
+    <row r="271" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A271" s="7"/>
       <c r="B271" s="7"/>
       <c r="C271" s="7"/>
@@ -7537,8 +7820,9 @@
       <c r="U271" s="7"/>
       <c r="V271" s="7"/>
       <c r="W271" s="7"/>
-    </row>
-    <row r="272" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X271" s="7"/>
+    </row>
+    <row r="272" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A272" s="7"/>
       <c r="B272" s="7"/>
       <c r="C272" s="7"/>
@@ -7562,8 +7846,9 @@
       <c r="U272" s="7"/>
       <c r="V272" s="7"/>
       <c r="W272" s="7"/>
-    </row>
-    <row r="273" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X272" s="7"/>
+    </row>
+    <row r="273" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A273" s="7"/>
       <c r="B273" s="7"/>
       <c r="C273" s="7"/>
@@ -7587,8 +7872,9 @@
       <c r="U273" s="7"/>
       <c r="V273" s="7"/>
       <c r="W273" s="7"/>
-    </row>
-    <row r="274" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X273" s="7"/>
+    </row>
+    <row r="274" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A274" s="7"/>
       <c r="B274" s="7"/>
       <c r="C274" s="7"/>
@@ -7612,8 +7898,9 @@
       <c r="U274" s="7"/>
       <c r="V274" s="7"/>
       <c r="W274" s="7"/>
-    </row>
-    <row r="275" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X274" s="7"/>
+    </row>
+    <row r="275" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A275" s="7"/>
       <c r="B275" s="7"/>
       <c r="C275" s="7"/>
@@ -7637,8 +7924,9 @@
       <c r="U275" s="7"/>
       <c r="V275" s="7"/>
       <c r="W275" s="7"/>
-    </row>
-    <row r="276" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X275" s="7"/>
+    </row>
+    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A276" s="7"/>
       <c r="B276" s="7"/>
       <c r="C276" s="7"/>
@@ -7662,8 +7950,9 @@
       <c r="U276" s="7"/>
       <c r="V276" s="7"/>
       <c r="W276" s="7"/>
-    </row>
-    <row r="277" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X276" s="7"/>
+    </row>
+    <row r="277" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A277" s="7"/>
       <c r="B277" s="7"/>
       <c r="C277" s="7"/>
@@ -7687,8 +7976,9 @@
       <c r="U277" s="7"/>
       <c r="V277" s="7"/>
       <c r="W277" s="7"/>
-    </row>
-    <row r="278" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X277" s="7"/>
+    </row>
+    <row r="278" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A278" s="7"/>
       <c r="B278" s="7"/>
       <c r="C278" s="7"/>
@@ -7712,8 +8002,9 @@
       <c r="U278" s="7"/>
       <c r="V278" s="7"/>
       <c r="W278" s="7"/>
-    </row>
-    <row r="279" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X278" s="7"/>
+    </row>
+    <row r="279" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A279" s="7"/>
       <c r="B279" s="7"/>
       <c r="C279" s="7"/>
@@ -7737,8 +8028,9 @@
       <c r="U279" s="7"/>
       <c r="V279" s="7"/>
       <c r="W279" s="7"/>
-    </row>
-    <row r="280" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X279" s="7"/>
+    </row>
+    <row r="280" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A280" s="7"/>
       <c r="B280" s="7"/>
       <c r="C280" s="7"/>
@@ -7762,8 +8054,9 @@
       <c r="U280" s="7"/>
       <c r="V280" s="7"/>
       <c r="W280" s="7"/>
-    </row>
-    <row r="281" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X280" s="7"/>
+    </row>
+    <row r="281" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A281" s="7"/>
       <c r="B281" s="7"/>
       <c r="C281" s="7"/>
@@ -7787,8 +8080,9 @@
       <c r="U281" s="7"/>
       <c r="V281" s="7"/>
       <c r="W281" s="7"/>
-    </row>
-    <row r="282" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X281" s="7"/>
+    </row>
+    <row r="282" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A282" s="7"/>
       <c r="B282" s="7"/>
       <c r="C282" s="7"/>
@@ -7812,8 +8106,9 @@
       <c r="U282" s="7"/>
       <c r="V282" s="7"/>
       <c r="W282" s="7"/>
-    </row>
-    <row r="283" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X282" s="7"/>
+    </row>
+    <row r="283" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A283" s="7"/>
       <c r="B283" s="7"/>
       <c r="C283" s="7"/>
@@ -7837,8 +8132,9 @@
       <c r="U283" s="7"/>
       <c r="V283" s="7"/>
       <c r="W283" s="7"/>
-    </row>
-    <row r="284" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X283" s="7"/>
+    </row>
+    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A284" s="7"/>
       <c r="B284" s="7"/>
       <c r="C284" s="7"/>
@@ -7862,8 +8158,9 @@
       <c r="U284" s="7"/>
       <c r="V284" s="7"/>
       <c r="W284" s="7"/>
-    </row>
-    <row r="285" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X284" s="7"/>
+    </row>
+    <row r="285" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A285" s="7"/>
       <c r="B285" s="7"/>
       <c r="C285" s="7"/>
@@ -7887,8 +8184,9 @@
       <c r="U285" s="7"/>
       <c r="V285" s="7"/>
       <c r="W285" s="7"/>
-    </row>
-    <row r="286" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X285" s="7"/>
+    </row>
+    <row r="286" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A286" s="7"/>
       <c r="B286" s="7"/>
       <c r="C286" s="7"/>
@@ -7912,8 +8210,9 @@
       <c r="U286" s="7"/>
       <c r="V286" s="7"/>
       <c r="W286" s="7"/>
-    </row>
-    <row r="287" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X286" s="7"/>
+    </row>
+    <row r="287" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A287" s="7"/>
       <c r="B287" s="7"/>
       <c r="C287" s="7"/>
@@ -7937,8 +8236,9 @@
       <c r="U287" s="7"/>
       <c r="V287" s="7"/>
       <c r="W287" s="7"/>
-    </row>
-    <row r="288" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X287" s="7"/>
+    </row>
+    <row r="288" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A288" s="7"/>
       <c r="B288" s="7"/>
       <c r="C288" s="7"/>
@@ -7962,8 +8262,9 @@
       <c r="U288" s="7"/>
       <c r="V288" s="7"/>
       <c r="W288" s="7"/>
-    </row>
-    <row r="289" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X288" s="7"/>
+    </row>
+    <row r="289" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A289" s="7"/>
       <c r="B289" s="7"/>
       <c r="C289" s="7"/>
@@ -7987,8 +8288,9 @@
       <c r="U289" s="7"/>
       <c r="V289" s="7"/>
       <c r="W289" s="7"/>
-    </row>
-    <row r="290" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X289" s="7"/>
+    </row>
+    <row r="290" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A290" s="7"/>
       <c r="B290" s="7"/>
       <c r="C290" s="7"/>
@@ -8012,8 +8314,9 @@
       <c r="U290" s="7"/>
       <c r="V290" s="7"/>
       <c r="W290" s="7"/>
-    </row>
-    <row r="291" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X290" s="7"/>
+    </row>
+    <row r="291" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A291" s="7"/>
       <c r="B291" s="7"/>
       <c r="C291" s="7"/>
@@ -8037,8 +8340,9 @@
       <c r="U291" s="7"/>
       <c r="V291" s="7"/>
       <c r="W291" s="7"/>
-    </row>
-    <row r="292" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X291" s="7"/>
+    </row>
+    <row r="292" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A292" s="7"/>
       <c r="B292" s="7"/>
       <c r="C292" s="7"/>
@@ -8062,8 +8366,9 @@
       <c r="U292" s="7"/>
       <c r="V292" s="7"/>
       <c r="W292" s="7"/>
-    </row>
-    <row r="293" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X292" s="7"/>
+    </row>
+    <row r="293" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A293" s="7"/>
       <c r="B293" s="7"/>
       <c r="C293" s="7"/>
@@ -8087,8 +8392,9 @@
       <c r="U293" s="7"/>
       <c r="V293" s="7"/>
       <c r="W293" s="7"/>
-    </row>
-    <row r="294" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X293" s="7"/>
+    </row>
+    <row r="294" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A294" s="7"/>
       <c r="B294" s="7"/>
       <c r="C294" s="7"/>
@@ -8112,8 +8418,9 @@
       <c r="U294" s="7"/>
       <c r="V294" s="7"/>
       <c r="W294" s="7"/>
-    </row>
-    <row r="295" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X294" s="7"/>
+    </row>
+    <row r="295" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A295" s="7"/>
       <c r="B295" s="7"/>
       <c r="C295" s="7"/>
@@ -8137,8 +8444,9 @@
       <c r="U295" s="7"/>
       <c r="V295" s="7"/>
       <c r="W295" s="7"/>
-    </row>
-    <row r="296" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X295" s="7"/>
+    </row>
+    <row r="296" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A296" s="7"/>
       <c r="B296" s="7"/>
       <c r="C296" s="7"/>
@@ -8162,8 +8470,9 @@
       <c r="U296" s="7"/>
       <c r="V296" s="7"/>
       <c r="W296" s="7"/>
-    </row>
-    <row r="297" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X296" s="7"/>
+    </row>
+    <row r="297" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A297" s="7"/>
       <c r="B297" s="7"/>
       <c r="C297" s="7"/>
@@ -8187,8 +8496,9 @@
       <c r="U297" s="7"/>
       <c r="V297" s="7"/>
       <c r="W297" s="7"/>
-    </row>
-    <row r="298" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X297" s="7"/>
+    </row>
+    <row r="298" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A298" s="7"/>
       <c r="B298" s="7"/>
       <c r="C298" s="7"/>
@@ -8212,8 +8522,9 @@
       <c r="U298" s="7"/>
       <c r="V298" s="7"/>
       <c r="W298" s="7"/>
-    </row>
-    <row r="299" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X298" s="7"/>
+    </row>
+    <row r="299" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A299" s="7"/>
       <c r="B299" s="7"/>
       <c r="C299" s="7"/>
@@ -8237,8 +8548,9 @@
       <c r="U299" s="7"/>
       <c r="V299" s="7"/>
       <c r="W299" s="7"/>
-    </row>
-    <row r="300" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X299" s="7"/>
+    </row>
+    <row r="300" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A300" s="7"/>
       <c r="B300" s="7"/>
       <c r="C300" s="7"/>
@@ -8262,8 +8574,9 @@
       <c r="U300" s="7"/>
       <c r="V300" s="7"/>
       <c r="W300" s="7"/>
-    </row>
-    <row r="301" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X300" s="7"/>
+    </row>
+    <row r="301" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A301" s="7"/>
       <c r="B301" s="7"/>
       <c r="C301" s="7"/>
@@ -8287,8 +8600,9 @@
       <c r="U301" s="7"/>
       <c r="V301" s="7"/>
       <c r="W301" s="7"/>
-    </row>
-    <row r="302" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X301" s="7"/>
+    </row>
+    <row r="302" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A302" s="7"/>
       <c r="B302" s="7"/>
       <c r="C302" s="7"/>
@@ -8312,8 +8626,9 @@
       <c r="U302" s="7"/>
       <c r="V302" s="7"/>
       <c r="W302" s="7"/>
-    </row>
-    <row r="303" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X302" s="7"/>
+    </row>
+    <row r="303" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A303" s="7"/>
       <c r="B303" s="7"/>
       <c r="C303" s="7"/>
@@ -8337,8 +8652,9 @@
       <c r="U303" s="7"/>
       <c r="V303" s="7"/>
       <c r="W303" s="7"/>
-    </row>
-    <row r="304" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X303" s="7"/>
+    </row>
+    <row r="304" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A304" s="7"/>
       <c r="B304" s="7"/>
       <c r="C304" s="7"/>
@@ -8362,8 +8678,9 @@
       <c r="U304" s="7"/>
       <c r="V304" s="7"/>
       <c r="W304" s="7"/>
-    </row>
-    <row r="305" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X304" s="7"/>
+    </row>
+    <row r="305" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A305" s="7"/>
       <c r="B305" s="7"/>
       <c r="C305" s="7"/>
@@ -8387,8 +8704,9 @@
       <c r="U305" s="7"/>
       <c r="V305" s="7"/>
       <c r="W305" s="7"/>
-    </row>
-    <row r="306" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X305" s="7"/>
+    </row>
+    <row r="306" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A306" s="7"/>
       <c r="B306" s="7"/>
       <c r="C306" s="7"/>
@@ -8412,8 +8730,9 @@
       <c r="U306" s="7"/>
       <c r="V306" s="7"/>
       <c r="W306" s="7"/>
-    </row>
-    <row r="307" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X306" s="7"/>
+    </row>
+    <row r="307" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A307" s="7"/>
       <c r="B307" s="7"/>
       <c r="C307" s="7"/>
@@ -8437,8 +8756,9 @@
       <c r="U307" s="7"/>
       <c r="V307" s="7"/>
       <c r="W307" s="7"/>
-    </row>
-    <row r="308" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X307" s="7"/>
+    </row>
+    <row r="308" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A308" s="7"/>
       <c r="B308" s="7"/>
       <c r="C308" s="7"/>
@@ -8462,8 +8782,9 @@
       <c r="U308" s="7"/>
       <c r="V308" s="7"/>
       <c r="W308" s="7"/>
-    </row>
-    <row r="309" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X308" s="7"/>
+    </row>
+    <row r="309" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A309" s="7"/>
       <c r="B309" s="7"/>
       <c r="C309" s="7"/>
@@ -8487,8 +8808,9 @@
       <c r="U309" s="7"/>
       <c r="V309" s="7"/>
       <c r="W309" s="7"/>
-    </row>
-    <row r="310" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X309" s="7"/>
+    </row>
+    <row r="310" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A310" s="7"/>
       <c r="B310" s="7"/>
       <c r="C310" s="7"/>
@@ -8512,8 +8834,9 @@
       <c r="U310" s="7"/>
       <c r="V310" s="7"/>
       <c r="W310" s="7"/>
-    </row>
-    <row r="311" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X310" s="7"/>
+    </row>
+    <row r="311" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A311" s="7"/>
       <c r="B311" s="7"/>
       <c r="C311" s="7"/>
@@ -8537,8 +8860,9 @@
       <c r="U311" s="7"/>
       <c r="V311" s="7"/>
       <c r="W311" s="7"/>
-    </row>
-    <row r="312" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X311" s="7"/>
+    </row>
+    <row r="312" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A312" s="7"/>
       <c r="B312" s="7"/>
       <c r="C312" s="7"/>
@@ -8562,8 +8886,9 @@
       <c r="U312" s="7"/>
       <c r="V312" s="7"/>
       <c r="W312" s="7"/>
-    </row>
-    <row r="313" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X312" s="7"/>
+    </row>
+    <row r="313" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A313" s="7"/>
       <c r="B313" s="7"/>
       <c r="C313" s="7"/>
@@ -8587,8 +8912,9 @@
       <c r="U313" s="7"/>
       <c r="V313" s="7"/>
       <c r="W313" s="7"/>
-    </row>
-    <row r="314" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X313" s="7"/>
+    </row>
+    <row r="314" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A314" s="7"/>
       <c r="B314" s="7"/>
       <c r="C314" s="7"/>
@@ -8612,8 +8938,9 @@
       <c r="U314" s="7"/>
       <c r="V314" s="7"/>
       <c r="W314" s="7"/>
-    </row>
-    <row r="315" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X314" s="7"/>
+    </row>
+    <row r="315" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A315" s="7"/>
       <c r="B315" s="7"/>
       <c r="C315" s="7"/>
@@ -8637,8 +8964,9 @@
       <c r="U315" s="7"/>
       <c r="V315" s="7"/>
       <c r="W315" s="7"/>
-    </row>
-    <row r="316" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X315" s="7"/>
+    </row>
+    <row r="316" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A316" s="7"/>
       <c r="B316" s="7"/>
       <c r="C316" s="7"/>
@@ -8662,8 +8990,9 @@
       <c r="U316" s="7"/>
       <c r="V316" s="7"/>
       <c r="W316" s="7"/>
-    </row>
-    <row r="317" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X316" s="7"/>
+    </row>
+    <row r="317" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A317" s="7"/>
       <c r="B317" s="7"/>
       <c r="C317" s="7"/>
@@ -8687,8 +9016,9 @@
       <c r="U317" s="7"/>
       <c r="V317" s="7"/>
       <c r="W317" s="7"/>
-    </row>
-    <row r="318" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X317" s="7"/>
+    </row>
+    <row r="318" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A318" s="7"/>
       <c r="B318" s="7"/>
       <c r="C318" s="7"/>
@@ -8712,8 +9042,9 @@
       <c r="U318" s="7"/>
       <c r="V318" s="7"/>
       <c r="W318" s="7"/>
-    </row>
-    <row r="319" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X318" s="7"/>
+    </row>
+    <row r="319" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A319" s="7"/>
       <c r="B319" s="7"/>
       <c r="C319" s="7"/>
@@ -8737,8 +9068,9 @@
       <c r="U319" s="7"/>
       <c r="V319" s="7"/>
       <c r="W319" s="7"/>
-    </row>
-    <row r="320" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X319" s="7"/>
+    </row>
+    <row r="320" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A320" s="7"/>
       <c r="B320" s="7"/>
       <c r="C320" s="7"/>
@@ -8762,8 +9094,9 @@
       <c r="U320" s="7"/>
       <c r="V320" s="7"/>
       <c r="W320" s="7"/>
-    </row>
-    <row r="321" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X320" s="7"/>
+    </row>
+    <row r="321" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A321" s="7"/>
       <c r="B321" s="7"/>
       <c r="C321" s="7"/>
@@ -8787,8 +9120,9 @@
       <c r="U321" s="7"/>
       <c r="V321" s="7"/>
       <c r="W321" s="7"/>
-    </row>
-    <row r="322" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X321" s="7"/>
+    </row>
+    <row r="322" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A322" s="7"/>
       <c r="B322" s="7"/>
       <c r="C322" s="7"/>
@@ -8812,8 +9146,9 @@
       <c r="U322" s="7"/>
       <c r="V322" s="7"/>
       <c r="W322" s="7"/>
-    </row>
-    <row r="323" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X322" s="7"/>
+    </row>
+    <row r="323" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A323" s="7"/>
       <c r="B323" s="7"/>
       <c r="C323" s="7"/>
@@ -8837,8 +9172,9 @@
       <c r="U323" s="7"/>
       <c r="V323" s="7"/>
       <c r="W323" s="7"/>
-    </row>
-    <row r="324" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X323" s="7"/>
+    </row>
+    <row r="324" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A324" s="7"/>
       <c r="B324" s="7"/>
       <c r="C324" s="7"/>
@@ -8862,8 +9198,9 @@
       <c r="U324" s="7"/>
       <c r="V324" s="7"/>
       <c r="W324" s="7"/>
-    </row>
-    <row r="325" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X324" s="7"/>
+    </row>
+    <row r="325" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A325" s="7"/>
       <c r="B325" s="7"/>
       <c r="C325" s="7"/>
@@ -8887,8 +9224,9 @@
       <c r="U325" s="7"/>
       <c r="V325" s="7"/>
       <c r="W325" s="7"/>
-    </row>
-    <row r="326" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X325" s="7"/>
+    </row>
+    <row r="326" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A326" s="7"/>
       <c r="B326" s="7"/>
       <c r="C326" s="7"/>
@@ -8912,8 +9250,9 @@
       <c r="U326" s="7"/>
       <c r="V326" s="7"/>
       <c r="W326" s="7"/>
-    </row>
-    <row r="327" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X326" s="7"/>
+    </row>
+    <row r="327" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A327" s="7"/>
       <c r="B327" s="7"/>
       <c r="C327" s="7"/>
@@ -8937,8 +9276,9 @@
       <c r="U327" s="7"/>
       <c r="V327" s="7"/>
       <c r="W327" s="7"/>
-    </row>
-    <row r="328" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X327" s="7"/>
+    </row>
+    <row r="328" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A328" s="7"/>
       <c r="B328" s="7"/>
       <c r="C328" s="7"/>
@@ -8962,8 +9302,9 @@
       <c r="U328" s="7"/>
       <c r="V328" s="7"/>
       <c r="W328" s="7"/>
-    </row>
-    <row r="329" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X328" s="7"/>
+    </row>
+    <row r="329" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A329" s="7"/>
       <c r="B329" s="7"/>
       <c r="C329" s="7"/>
@@ -8987,8 +9328,9 @@
       <c r="U329" s="7"/>
       <c r="V329" s="7"/>
       <c r="W329" s="7"/>
-    </row>
-    <row r="330" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X329" s="7"/>
+    </row>
+    <row r="330" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A330" s="7"/>
       <c r="B330" s="7"/>
       <c r="C330" s="7"/>
@@ -9012,8 +9354,9 @@
       <c r="U330" s="7"/>
       <c r="V330" s="7"/>
       <c r="W330" s="7"/>
-    </row>
-    <row r="331" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X330" s="7"/>
+    </row>
+    <row r="331" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A331" s="7"/>
       <c r="B331" s="7"/>
       <c r="C331" s="7"/>
@@ -9037,8 +9380,9 @@
       <c r="U331" s="7"/>
       <c r="V331" s="7"/>
       <c r="W331" s="7"/>
-    </row>
-    <row r="332" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X331" s="7"/>
+    </row>
+    <row r="332" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A332" s="7"/>
       <c r="B332" s="7"/>
       <c r="C332" s="7"/>
@@ -9062,8 +9406,9 @@
       <c r="U332" s="7"/>
       <c r="V332" s="7"/>
       <c r="W332" s="7"/>
-    </row>
-    <row r="333" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X332" s="7"/>
+    </row>
+    <row r="333" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A333" s="7"/>
       <c r="B333" s="7"/>
       <c r="C333" s="7"/>
@@ -9087,8 +9432,9 @@
       <c r="U333" s="7"/>
       <c r="V333" s="7"/>
       <c r="W333" s="7"/>
-    </row>
-    <row r="334" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X333" s="7"/>
+    </row>
+    <row r="334" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A334" s="7"/>
       <c r="B334" s="7"/>
       <c r="C334" s="7"/>
@@ -9112,8 +9458,9 @@
       <c r="U334" s="7"/>
       <c r="V334" s="7"/>
       <c r="W334" s="7"/>
-    </row>
-    <row r="335" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X334" s="7"/>
+    </row>
+    <row r="335" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A335" s="7"/>
       <c r="B335" s="7"/>
       <c r="C335" s="7"/>
@@ -9137,9 +9484,16 @@
       <c r="U335" s="7"/>
       <c r="V335" s="7"/>
       <c r="W335" s="7"/>
+      <c r="X335" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="G1:G2"/>
@@ -9148,12 +9502,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9162,21 +9510,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A19:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="6.375" style="8" customWidth="1"/>
+    <col min="1" max="2" width="6.33203125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9185,12 +9533,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>